<commit_message>
Se agrega modulo de Asistencias
</commit_message>
<xml_diff>
--- a/EstadoPruebaProyectoIntegrador.xlsx
+++ b/EstadoPruebaProyectoIntegrador.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JM\ControlPruebaProyectoIntegrador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89185ACB-3849-4D68-9F35-092028C3A7C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CC6BFB-0E70-47E8-B6C2-05E6438F76AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="161">
   <si>
     <t>PRUEBA PROYECTO INTEGRADOR</t>
   </si>
@@ -505,6 +505,9 @@
   </si>
   <si>
     <t>Integrar panel general de indicadores</t>
+  </si>
+  <si>
+    <t>Asistencia</t>
   </si>
 </sst>
 </file>
@@ -579,82 +582,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="17">
     <dxf>
       <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-          <stop position="0.5">
-            <color theme="9" tint="0.40000610370189521"/>
-          </stop>
-          <stop position="1">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-          <stop position="0.5">
-            <color theme="7" tint="0.59999389629810485"/>
-          </stop>
-          <stop position="1">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-          <stop position="0.5">
-            <color theme="5" tint="0.80001220740379042"/>
-          </stop>
-          <stop position="1">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="0.5">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-          <stop position="1">
-            <color theme="0"/>
-          </stop>
-        </gradientFill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
       </fill>
     </dxf>
     <dxf>
@@ -666,9 +613,17 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="0.5">
+            <color theme="2" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
       </fill>
     </dxf>
     <dxf>
@@ -678,7 +633,37 @@
             <color theme="2" tint="-0.25098422193060094"/>
           </stop>
           <stop position="0.5">
-            <color theme="4"/>
+            <color theme="5" tint="0.80001220740379042"/>
+          </stop>
+          <stop position="1">
+            <color theme="2" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="2" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="0.5">
+            <color theme="7" tint="0.59999389629810485"/>
+          </stop>
+          <stop position="1">
+            <color theme="2" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="2" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="0.5">
+            <color theme="9" tint="0.40000610370189521"/>
           </stop>
           <stop position="1">
             <color theme="2" tint="-0.25098422193060094"/>
@@ -708,10 +693,40 @@
             <color theme="2" tint="-0.25098422193060094"/>
           </stop>
           <stop position="0.5">
-            <color theme="9" tint="0.40000610370189521"/>
+            <color theme="4"/>
           </stop>
           <stop position="1">
             <color theme="2" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="9" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="0.5">
+            <color theme="2" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="1">
+            <color theme="9" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="0.5">
+            <color theme="2" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
           </stop>
         </gradientFill>
       </fill>
@@ -723,7 +738,7 @@
             <color theme="2" tint="-0.25098422193060094"/>
           </stop>
           <stop position="0.5">
-            <color theme="7" tint="0.59999389629810485"/>
+            <color theme="5" tint="0.80001220740379042"/>
           </stop>
           <stop position="1">
             <color theme="2" tint="-0.25098422193060094"/>
@@ -738,7 +753,7 @@
             <color theme="2" tint="-0.25098422193060094"/>
           </stop>
           <stop position="0.5">
-            <color theme="5" tint="0.80001220740379042"/>
+            <color theme="7" tint="0.59999389629810485"/>
           </stop>
           <stop position="1">
             <color theme="2" tint="-0.25098422193060094"/>
@@ -750,22 +765,30 @@
       <fill>
         <gradientFill degree="90">
           <stop position="0">
-            <color theme="0"/>
+            <color theme="2" tint="-0.25098422193060094"/>
           </stop>
           <stop position="0.5">
+            <color theme="9" tint="0.40000610370189521"/>
+          </stop>
+          <stop position="1">
             <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-          <stop position="1">
-            <color theme="0"/>
           </stop>
         </gradientFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="9" tint="0.40000610370189521"/>
+          </stop>
+          <stop position="0.5">
+            <color theme="7" tint="0.40000610370189521"/>
+          </stop>
+          <stop position="1">
+            <color theme="9" tint="0.40000610370189521"/>
+          </stop>
+        </gradientFill>
       </fill>
     </dxf>
     <dxf>
@@ -777,164 +800,8 @@
     </dxf>
     <dxf>
       <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-          <stop position="0.5">
-            <color theme="4"/>
-          </stop>
-          <stop position="1">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-          <stop position="0.5">
-            <color theme="8" tint="0.40000610370189521"/>
-          </stop>
-          <stop position="1">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-          <stop position="0.5">
-            <color theme="7" tint="0.59999389629810485"/>
-          </stop>
-          <stop position="1">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-          <stop position="0.5">
-            <color theme="5" tint="0.80001220740379042"/>
-          </stop>
-          <stop position="1">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="0.5">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-          <stop position="1">
-            <color theme="0"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-          <stop position="0.5">
-            <color theme="4"/>
-          </stop>
-          <stop position="1">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-          <stop position="0.5">
-            <color theme="7" tint="0.59999389629810485"/>
-          </stop>
-          <stop position="1">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-          <stop position="0.5">
-            <color theme="5" tint="0.80001220740379042"/>
-          </stop>
-          <stop position="1">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="0.5">
-            <color theme="2" tint="-0.25098422193060094"/>
-          </stop>
-          <stop position="1">
-            <color theme="0"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1231,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G184"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D8"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="F143" sqref="F143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,24 +1112,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1293,7 +1160,7 @@
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G4" t="s">
@@ -1310,7 +1177,7 @@
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G5" t="s">
@@ -1327,7 +1194,7 @@
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1341,7 +1208,7 @@
       <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1355,7 +1222,7 @@
       <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1576,10 +1443,10 @@
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1588,7 +1455,7 @@
       <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -1602,7 +1469,7 @@
       <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1616,7 +1483,7 @@
       <c r="B28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1630,7 +1497,7 @@
       <c r="B29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1644,7 +1511,7 @@
       <c r="B30" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -1658,7 +1525,7 @@
       <c r="B31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1672,7 +1539,7 @@
       <c r="B32" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1686,7 +1553,7 @@
       <c r="B33" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -1700,7 +1567,7 @@
       <c r="B34" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1714,7 +1581,7 @@
       <c r="B35" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1728,7 +1595,7 @@
       <c r="B36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1742,7 +1609,7 @@
       <c r="B37" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -1756,7 +1623,7 @@
       <c r="B38" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1770,7 +1637,7 @@
       <c r="B39" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -1784,7 +1651,7 @@
       <c r="B40" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -1798,7 +1665,7 @@
       <c r="B41" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -1812,7 +1679,7 @@
       <c r="B42" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -1826,7 +1693,7 @@
       <c r="B43" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -1840,7 +1707,7 @@
       <c r="B44" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -1854,7 +1721,7 @@
       <c r="B45" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1868,10 +1735,10 @@
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -1880,7 +1747,7 @@
       <c r="B48" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -1888,1468 +1755,1628 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D68" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
+      <c r="A69" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
-      <c r="B71" s="6"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
+      <c r="A72" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C72" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C73" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D73" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C74" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
+      <c r="A75" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C75" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
+      <c r="A76" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C76" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
+      <c r="A77" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
+      <c r="A78" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C78" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="C79" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D79" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
+      <c r="A80" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="C80" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="D80" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="C81" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
+      <c r="A82" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="C82" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D82" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
+      <c r="A83" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C83" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D83" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
+      <c r="A84" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="C84" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C85" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D85" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
+      <c r="A86" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C86" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="D86" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
+      <c r="A87" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="C87" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D87" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
+      <c r="A88" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="C88" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C89" s="5" t="s">
+      <c r="C89" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="D89" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
+      <c r="A90" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C90" s="5" t="s">
+      <c r="C90" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="D90" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
+      <c r="A91" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C91" s="5" t="s">
+      <c r="C91" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="D91" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="6"/>
-      <c r="B93" s="6"/>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C94" s="5" t="s">
+      <c r="C94" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D94" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
+      <c r="A95" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="C95" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D95" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
+      <c r="A96" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C96" s="5" t="s">
+      <c r="C96" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D96" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
+      <c r="A97" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C97" s="5" t="s">
+      <c r="C97" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="D97" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
+      <c r="A98" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B98" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C98" s="5" t="s">
+      <c r="C98" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="D98" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
+      <c r="A99" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B99" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C99" s="5" t="s">
+      <c r="C99" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="D99" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="5" t="s">
+      <c r="A100" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B100" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C100" s="5" t="s">
+      <c r="C100" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D100" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
+      <c r="A101" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C101" s="5" t="s">
+      <c r="C101" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="D101" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
+      <c r="A102" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C102" s="5" t="s">
+      <c r="C102" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D102" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
+      <c r="A103" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C103" s="5" t="s">
+      <c r="C103" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="D103" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
+      <c r="A104" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B104" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C104" s="5" t="s">
+      <c r="C104" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D104" s="5" t="s">
+      <c r="D104" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
+      <c r="A105" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B105" s="5" t="s">
+      <c r="B105" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C105" s="5" t="s">
+      <c r="C105" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D105" s="5" t="s">
+      <c r="D105" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
+      <c r="A106" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B106" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C106" s="5" t="s">
+      <c r="C106" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D106" s="5" t="s">
+      <c r="D106" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
+      <c r="A107" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="B107" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C107" s="5" t="s">
+      <c r="C107" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D107" s="5" t="s">
+      <c r="D107" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
+      <c r="A108" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="B108" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C108" s="5" t="s">
+      <c r="C108" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D108" s="5" t="s">
+      <c r="D108" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="5" t="s">
+      <c r="A109" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="B109" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C109" s="5" t="s">
+      <c r="C109" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D109" s="5" t="s">
+      <c r="D109" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
+      <c r="A110" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B110" s="5" t="s">
+      <c r="B110" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C110" s="5" t="s">
+      <c r="C110" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D110" s="5" t="s">
+      <c r="D110" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
+      <c r="A111" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B111" s="5" t="s">
+      <c r="B111" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C111" s="5" t="s">
+      <c r="C111" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D111" s="5" t="s">
+      <c r="D111" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="5" t="s">
+      <c r="A112" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B112" s="5" t="s">
+      <c r="B112" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C112" s="5" t="s">
+      <c r="C112" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D112" s="5" t="s">
+      <c r="D112" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="5" t="s">
+      <c r="A113" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B113" s="5" t="s">
+      <c r="B113" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C113" s="5" t="s">
+      <c r="C113" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D113" s="5" t="s">
+      <c r="D113" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="5"/>
-      <c r="B114" s="5"/>
-      <c r="C114" s="5"/>
-      <c r="D114" s="5"/>
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="6"/>
-      <c r="B115" s="6"/>
-      <c r="C115" s="6"/>
-      <c r="D115" s="6"/>
+      <c r="A115" s="3"/>
+      <c r="B115" s="3"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="5" t="s">
+      <c r="A116" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B116" s="5" t="s">
+      <c r="B116" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C116" s="7" t="s">
+      <c r="C116" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D116" s="5" t="s">
+      <c r="D116" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="5" t="s">
+      <c r="A117" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B117" s="5" t="s">
+      <c r="B117" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C117" s="7" t="s">
+      <c r="C117" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D117" s="5" t="s">
+      <c r="D117" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="5" t="s">
+      <c r="A118" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B118" s="5" t="s">
+      <c r="B118" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C118" s="7" t="s">
+      <c r="C118" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D118" s="5" t="s">
+      <c r="D118" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="5" t="s">
+      <c r="A119" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B119" s="5" t="s">
+      <c r="B119" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C119" s="7" t="s">
+      <c r="C119" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D119" s="5" t="s">
+      <c r="D119" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="5" t="s">
+      <c r="A120" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B120" s="5" t="s">
+      <c r="B120" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C120" s="7" t="s">
+      <c r="C120" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D120" s="5" t="s">
+      <c r="D120" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="5" t="s">
+      <c r="A121" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B121" s="5" t="s">
+      <c r="B121" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C121" s="7" t="s">
+      <c r="C121" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D121" s="5" t="s">
+      <c r="D121" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="5" t="s">
+      <c r="A122" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B122" s="5" t="s">
+      <c r="B122" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C122" s="7" t="s">
+      <c r="C122" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D122" s="5" t="s">
+      <c r="D122" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="5" t="s">
+      <c r="A123" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B123" s="5" t="s">
+      <c r="B123" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C123" s="7" t="s">
+      <c r="C123" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D123" s="5" t="s">
+      <c r="D123" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="5" t="s">
+      <c r="A124" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B124" s="5" t="s">
+      <c r="B124" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C124" s="7" t="s">
+      <c r="C124" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D124" s="5" t="s">
+      <c r="D124" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="5" t="s">
+      <c r="A125" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B125" s="5" t="s">
+      <c r="B125" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C125" s="7" t="s">
+      <c r="C125" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D125" s="5" t="s">
+      <c r="D125" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="5" t="s">
+      <c r="A126" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B126" s="5" t="s">
+      <c r="B126" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C126" s="7" t="s">
+      <c r="C126" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D126" s="5" t="s">
+      <c r="D126" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="5" t="s">
+      <c r="A127" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B127" s="5" t="s">
+      <c r="B127" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C127" s="7" t="s">
+      <c r="C127" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D127" s="5" t="s">
+      <c r="D127" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="5" t="s">
+      <c r="A128" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B128" s="5" t="s">
+      <c r="B128" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C128" s="7" t="s">
+      <c r="C128" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D128" s="5" t="s">
+      <c r="D128" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="5" t="s">
+      <c r="A129" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B129" s="5" t="s">
+      <c r="B129" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C129" s="7" t="s">
+      <c r="C129" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D129" s="5" t="s">
+      <c r="D129" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="5" t="s">
+      <c r="A130" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B130" s="5" t="s">
+      <c r="B130" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C130" s="7" t="s">
+      <c r="C130" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D130" s="5" t="s">
+      <c r="D130" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="5" t="s">
+      <c r="A131" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B131" s="5" t="s">
+      <c r="B131" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C131" s="7" t="s">
+      <c r="C131" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D131" s="5" t="s">
+      <c r="D131" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="5" t="s">
+      <c r="A132" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B132" s="5" t="s">
+      <c r="B132" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C132" s="7" t="s">
+      <c r="C132" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D132" s="5" t="s">
+      <c r="D132" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="5" t="s">
+      <c r="A133" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B133" s="5" t="s">
+      <c r="B133" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C133" s="7" t="s">
+      <c r="C133" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D133" s="5" t="s">
+      <c r="D133" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="5" t="s">
+      <c r="A134" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B134" s="5" t="s">
+      <c r="B134" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C134" s="7" t="s">
+      <c r="C134" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D134" s="5" t="s">
+      <c r="D134" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="5" t="s">
+      <c r="A135" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B135" s="5" t="s">
+      <c r="B135" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C135" s="7" t="s">
+      <c r="C135" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D135" s="5" t="s">
+      <c r="D135" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="5"/>
-      <c r="B136" s="5"/>
-      <c r="C136" s="5"/>
-      <c r="D136" s="5"/>
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+      <c r="C136" s="1"/>
+      <c r="D136" s="1"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="5"/>
-      <c r="B137" s="5"/>
-      <c r="C137" s="5"/>
-      <c r="D137" s="5"/>
+      <c r="A137" s="3"/>
+      <c r="B137" s="3"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="5"/>
-      <c r="B138" s="5"/>
-      <c r="C138" s="5"/>
-      <c r="D138" s="5"/>
+      <c r="A138" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="5"/>
-      <c r="B139" s="5"/>
-      <c r="C139" s="5"/>
-      <c r="D139" s="5"/>
+      <c r="A139" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="5"/>
-      <c r="B140" s="5"/>
-      <c r="C140" s="5"/>
-      <c r="D140" s="5"/>
+      <c r="A140" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="5"/>
-      <c r="B141" s="5"/>
-      <c r="C141" s="5"/>
-      <c r="D141" s="5"/>
+      <c r="A141" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="5"/>
-      <c r="B142" s="5"/>
-      <c r="C142" s="5"/>
-      <c r="D142" s="5"/>
+      <c r="A142" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="5"/>
-      <c r="B143" s="5"/>
-      <c r="C143" s="5"/>
-      <c r="D143" s="5"/>
+      <c r="A143" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="5"/>
-      <c r="B144" s="5"/>
-      <c r="C144" s="5"/>
-      <c r="D144" s="5"/>
+      <c r="A144" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="5"/>
-      <c r="B145" s="5"/>
-      <c r="C145" s="5"/>
-      <c r="D145" s="5"/>
+      <c r="A145" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="5"/>
-      <c r="B146" s="5"/>
-      <c r="C146" s="5"/>
-      <c r="D146" s="5"/>
+      <c r="A146" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="5"/>
-      <c r="B147" s="5"/>
-      <c r="C147" s="5"/>
-      <c r="D147" s="5"/>
+      <c r="A147" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="5"/>
-      <c r="B148" s="5"/>
-      <c r="C148" s="5"/>
-      <c r="D148" s="5"/>
+      <c r="A148" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="5"/>
-      <c r="B149" s="5"/>
-      <c r="C149" s="5"/>
-      <c r="D149" s="5"/>
+      <c r="A149" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="5"/>
-      <c r="B150" s="5"/>
-      <c r="C150" s="5"/>
-      <c r="D150" s="5"/>
+      <c r="A150" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="5"/>
-      <c r="B151" s="5"/>
-      <c r="C151" s="5"/>
-      <c r="D151" s="5"/>
+      <c r="A151" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="5"/>
-      <c r="B152" s="5"/>
-      <c r="C152" s="5"/>
-      <c r="D152" s="5"/>
+      <c r="A152" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="5"/>
-      <c r="B153" s="5"/>
-      <c r="C153" s="5"/>
-      <c r="D153" s="5"/>
+      <c r="A153" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="5"/>
-      <c r="B154" s="5"/>
-      <c r="C154" s="5"/>
-      <c r="D154" s="5"/>
+      <c r="A154" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="5"/>
-      <c r="B155" s="5"/>
-      <c r="C155" s="5"/>
-      <c r="D155" s="5"/>
+      <c r="A155" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="5"/>
-      <c r="B156" s="5"/>
-      <c r="C156" s="5"/>
-      <c r="D156" s="5"/>
+      <c r="A156" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="5"/>
-      <c r="B157" s="5"/>
-      <c r="C157" s="5"/>
-      <c r="D157" s="5"/>
+      <c r="A157" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="5"/>
-      <c r="B158" s="5"/>
-      <c r="C158" s="5"/>
-      <c r="D158" s="5"/>
+      <c r="A158" s="1"/>
+      <c r="B158" s="1"/>
+      <c r="C158" s="1"/>
+      <c r="D158" s="1"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="5"/>
-      <c r="B159" s="5"/>
-      <c r="C159" s="5"/>
-      <c r="D159" s="5"/>
+      <c r="A159" s="1"/>
+      <c r="B159" s="1"/>
+      <c r="C159" s="1"/>
+      <c r="D159" s="1"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="5"/>
-      <c r="B160" s="5"/>
-      <c r="C160" s="5"/>
-      <c r="D160" s="5"/>
+      <c r="A160" s="1"/>
+      <c r="B160" s="1"/>
+      <c r="C160" s="1"/>
+      <c r="D160" s="1"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="5"/>
-      <c r="B161" s="5"/>
-      <c r="C161" s="5"/>
-      <c r="D161" s="5"/>
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
+      <c r="C161" s="1"/>
+      <c r="D161" s="1"/>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="5"/>
-      <c r="B162" s="5"/>
-      <c r="C162" s="5"/>
-      <c r="D162" s="5"/>
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
+      <c r="C162" s="1"/>
+      <c r="D162" s="1"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="5"/>
-      <c r="B163" s="5"/>
-      <c r="C163" s="5"/>
-      <c r="D163" s="5"/>
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
+      <c r="C163" s="1"/>
+      <c r="D163" s="1"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="5"/>
-      <c r="B164" s="5"/>
-      <c r="C164" s="5"/>
-      <c r="D164" s="5"/>
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
+      <c r="C164" s="1"/>
+      <c r="D164" s="1"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="5"/>
-      <c r="B165" s="5"/>
-      <c r="C165" s="5"/>
-      <c r="D165" s="5"/>
+      <c r="A165" s="1"/>
+      <c r="B165" s="1"/>
+      <c r="C165" s="1"/>
+      <c r="D165" s="1"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="5"/>
-      <c r="B166" s="5"/>
-      <c r="C166" s="5"/>
-      <c r="D166" s="5"/>
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
+      <c r="C166" s="1"/>
+      <c r="D166" s="1"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="5"/>
-      <c r="B167" s="5"/>
-      <c r="C167" s="5"/>
-      <c r="D167" s="5"/>
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
+      <c r="C167" s="1"/>
+      <c r="D167" s="1"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="5"/>
-      <c r="B168" s="5"/>
-      <c r="C168" s="5"/>
-      <c r="D168" s="5"/>
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
+      <c r="C168" s="1"/>
+      <c r="D168" s="1"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="5"/>
-      <c r="B169" s="5"/>
-      <c r="C169" s="5"/>
-      <c r="D169" s="5"/>
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
+      <c r="C169" s="1"/>
+      <c r="D169" s="1"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="5"/>
-      <c r="B170" s="5"/>
-      <c r="C170" s="5"/>
-      <c r="D170" s="5"/>
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
+      <c r="C170" s="1"/>
+      <c r="D170" s="1"/>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="5"/>
-      <c r="B171" s="5"/>
-      <c r="C171" s="5"/>
-      <c r="D171" s="5"/>
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="5"/>
-      <c r="B172" s="5"/>
-      <c r="C172" s="5"/>
-      <c r="D172" s="5"/>
+      <c r="A172" s="1"/>
+      <c r="B172" s="1"/>
+      <c r="C172" s="1"/>
+      <c r="D172" s="1"/>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="5"/>
-      <c r="B173" s="5"/>
-      <c r="C173" s="5"/>
-      <c r="D173" s="5"/>
+      <c r="A173" s="1"/>
+      <c r="B173" s="1"/>
+      <c r="C173" s="1"/>
+      <c r="D173" s="1"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="5"/>
-      <c r="B174" s="5"/>
-      <c r="C174" s="5"/>
-      <c r="D174" s="5"/>
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
+      <c r="C174" s="1"/>
+      <c r="D174" s="1"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="5"/>
-      <c r="B175" s="5"/>
-      <c r="C175" s="5"/>
-      <c r="D175" s="5"/>
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
+      <c r="C175" s="1"/>
+      <c r="D175" s="1"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="5"/>
-      <c r="B176" s="5"/>
-      <c r="C176" s="5"/>
-      <c r="D176" s="5"/>
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
+      <c r="C176" s="1"/>
+      <c r="D176" s="1"/>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="5"/>
-      <c r="B177" s="5"/>
-      <c r="C177" s="5"/>
-      <c r="D177" s="5"/>
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
+      <c r="C177" s="1"/>
+      <c r="D177" s="1"/>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="5"/>
-      <c r="B178" s="5"/>
-      <c r="C178" s="5"/>
-      <c r="D178" s="5"/>
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
+      <c r="C178" s="1"/>
+      <c r="D178" s="1"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="5"/>
-      <c r="B179" s="5"/>
-      <c r="C179" s="5"/>
-      <c r="D179" s="5"/>
+      <c r="A179" s="1"/>
+      <c r="B179" s="1"/>
+      <c r="C179" s="1"/>
+      <c r="D179" s="1"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="5"/>
-      <c r="B180" s="5"/>
-      <c r="C180" s="5"/>
-      <c r="D180" s="5"/>
+      <c r="A180" s="1"/>
+      <c r="B180" s="1"/>
+      <c r="C180" s="1"/>
+      <c r="D180" s="1"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="5"/>
-      <c r="B181" s="5"/>
-      <c r="C181" s="5"/>
-      <c r="D181" s="5"/>
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
+      <c r="C181" s="1"/>
+      <c r="D181" s="1"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="5"/>
-      <c r="B182" s="5"/>
-      <c r="C182" s="5"/>
-      <c r="D182" s="5"/>
+      <c r="A182" s="1"/>
+      <c r="B182" s="1"/>
+      <c r="C182" s="1"/>
+      <c r="D182" s="1"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="5"/>
-      <c r="B183" s="5"/>
-      <c r="C183" s="5"/>
-      <c r="D183" s="5"/>
+      <c r="A183" s="1"/>
+      <c r="B183" s="1"/>
+      <c r="C183" s="1"/>
+      <c r="D183" s="1"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="5"/>
-      <c r="B184" s="5"/>
-      <c r="C184" s="5"/>
-      <c r="D184" s="5"/>
+      <c r="A184" s="1"/>
+      <c r="B184" s="1"/>
+      <c r="C184" s="1"/>
+      <c r="D184" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3357,36 +3384,39 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A3:A23">
-    <cfRule type="containsText" dxfId="14" priority="9" operator="containsText" text="Ingreso y Registro">
+    <cfRule type="containsText" dxfId="16" priority="10" operator="containsText" text="Ingreso y Registro">
       <formula>NOT(ISERROR(SEARCH("Ingreso y Registro",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A1:D1048576">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+      <formula>"Estadistica"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+      <formula>"Apoyo estudiantil"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+      <formula>"Academico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+      <formula>"Familiar"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+      <formula>"Hoja de vida estudiantil"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>"Asistencia"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" priority="8" operator="equal">
-      <formula>"Pendiente"</formula>
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+      <formula>"Terminado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
       <formula>"En proceso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
-      <formula>"Terminado"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
-      <formula>"Hoja de vida estudiantil"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
-      <formula>"Familiar"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
-      <formula>"Academico"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
-      <formula>"Apoyo estudiantil"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
-      <formula>"Estadistica"</formula>
+    <cfRule type="cellIs" priority="9" operator="equal">
+      <formula>"Pendiente"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>